<commit_message>
Created Character and VisualCharacter class
Able to move and hit (with currently no other behaviour than play
animation)
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Daily total</t>
+  </si>
+  <si>
+    <t>Created basic scene and created Character with moves and hit</t>
   </si>
 </sst>
 </file>
@@ -56,7 +59,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -72,6 +75,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,6 +194,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -499,7 +511,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,17 +542,23 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="str">
+      <c r="B3" s="13">
+        <v>42311</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <f>IF(D3="", "", SUM(D$3:D3))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created GameManager and CharacterManager
Able to create heroes and catch inputs for the selected one (can't
switch hero yet and others don't follow selected one)
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Created basic scene and created Character with moves and hit</t>
+  </si>
+  <si>
+    <t>Created GameManager and CharacterManager with character creation and control logic</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -154,11 +157,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,6 +213,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -511,7 +530,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +561,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13">
+      <c r="B3" s="14">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -558,16 +577,20 @@
       <c r="F3" s="9"/>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="str">
+      <c r="B4" s="13"/>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
         <f>IF(D4="", "", SUM(D$3:D4))</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="F4" s="8"/>
     </row>
@@ -2532,6 +2555,9 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Now unselected characters follow the selected one
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Date</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Created GameManager and CharacterManager with character creation and control logic</t>
+  </si>
+  <si>
+    <t>Added camera follow + unselected characters now follow the selected one</t>
   </si>
 </sst>
 </file>
@@ -212,10 +215,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,7 +533,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,7 +564,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -577,11 +580,11 @@
       <c r="F3" s="9"/>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -595,12 +598,16 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="str">
+      <c r="B5" s="14"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="1">
         <f>IF(D5="", "", SUM(D$3:D5))</f>
-        <v/>
+        <v>3.5</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -2556,7 +2563,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Created ManaPanel, CharacterPanel and UIManager
Fully functionnal, except select hero
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -43,6 +43,9 @@
   <si>
     <t>Added camera follow + unselected characters now follow the selected one</t>
   </si>
+  <si>
+    <t>Created ManaPanel, CharacterPanel and UIManager + "designed" character panel -&gt; fully functionnal (except select hero)</t>
+  </si>
 </sst>
 </file>
 
@@ -65,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +90,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,6 +228,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,7 +548,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +595,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>3.5</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -598,7 +613,7 @@
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -612,12 +627,18 @@
       <c r="F5" s="8"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="str">
+      <c r="B6" s="16">
+        <v>42312</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1">
         <f>IF(D6="", "", SUM(D$3:D6))</f>
-        <v/>
+        <v>9.5</v>
       </c>
       <c r="F6" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added all weapons (+ Item.cs) and empty Armor.cs
Weapons are fully functionnal
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Created ManaPanel, CharacterPanel and UIManager + "designed" character panel -&gt; fully functionnal (except select hero)</t>
+  </si>
+  <si>
+    <t>Created InventoryPanel and basic logic (no Refresh yet)</t>
+  </si>
+  <si>
+    <t>Created Item.cs, Weapon.cs, Sword.cs, Bow.cs, Staff.cs and Arrow.cs (Fully functional)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,9 +218,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -222,6 +225,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -233,7 +239,25 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -548,7 +572,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,10 +616,13 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>1</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="18">
+        <f>SUM(D3:D5)</f>
+        <v>3.5</v>
+      </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>9.5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -610,7 +637,7 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>3</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
@@ -624,7 +651,7 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>3.5</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="22"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="16">
@@ -640,30 +667,43 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>9.5</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="20">
+        <f>SUM(D6:D7)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="str">
+      <c r="B7" s="17"/>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
         <f>IF(D7="", "", SUM(D$3:D7))</f>
-        <v/>
-      </c>
-      <c r="F7" s="8"/>
+        <v>10.5</v>
+      </c>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="str">
+      <c r="B8" s="12">
+        <v>42313</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
         <f>IF(D8="", "", SUM(D$3:D8))</f>
-        <v/>
+        <v>14.5</v>
       </c>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="str">
@@ -673,7 +713,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="4"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="str">
@@ -683,7 +723,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="str">
@@ -693,7 +733,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="4"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="str">
@@ -703,7 +743,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="4"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="str">
@@ -713,7 +753,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="str">
@@ -723,7 +763,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="str">
@@ -733,7 +773,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="4"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="str">
@@ -743,7 +783,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="4"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="str">
@@ -753,7 +793,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="4"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="str">
@@ -763,7 +803,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="4"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="str">
@@ -773,7 +813,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="4"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="str">
@@ -783,7 +823,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="4"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="str">
@@ -793,7 +833,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="4"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="str">
@@ -803,7 +843,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="4"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="str">
@@ -813,7 +853,7 @@
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="4"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="str">
@@ -823,7 +863,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="str">
@@ -833,7 +873,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="4"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="str">
@@ -843,7 +883,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="4"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="str">
@@ -853,7 +893,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="4"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="str">
@@ -863,7 +903,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="4"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="str">
@@ -873,7 +913,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="4"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="str">
@@ -883,7 +923,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="str">
@@ -893,7 +933,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="12"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="4"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="str">
@@ -903,7 +943,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="4"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="str">
@@ -913,7 +953,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="str">
@@ -923,7 +963,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
+      <c r="B35" s="11"/>
       <c r="C35" s="4"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="str">
@@ -933,7 +973,7 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
+      <c r="B36" s="11"/>
       <c r="C36" s="4"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="str">
@@ -943,14 +983,14 @@
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="12"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="str">
         <f>IF(D37="", "", SUM(D$3:D37))</f>
         <v/>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
@@ -1000,7 +1040,7 @@
         <f>IF(D42="", "", SUM(D$3:D42))</f>
         <v/>
       </c>
-      <c r="F42" s="10"/>
+      <c r="F42" s="9"/>
     </row>
     <row r="43" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
@@ -1010,7 +1050,7 @@
         <f>IF(D43="", "", SUM(D$3:D43))</f>
         <v/>
       </c>
-      <c r="F43" s="10"/>
+      <c r="F43" s="9"/>
     </row>
     <row r="44" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
@@ -1020,7 +1060,7 @@
         <f>IF(D44="", "", SUM(D$3:D44))</f>
         <v/>
       </c>
-      <c r="F44" s="10"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
@@ -1030,7 +1070,7 @@
         <f>IF(D45="", "", SUM(D$3:D45))</f>
         <v/>
       </c>
-      <c r="F45" s="10"/>
+      <c r="F45" s="9"/>
     </row>
     <row r="46" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
@@ -1040,7 +1080,7 @@
         <f>IF(D46="", "", SUM(D$3:D46))</f>
         <v/>
       </c>
-      <c r="F46" s="10"/>
+      <c r="F46" s="9"/>
     </row>
     <row r="47" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
@@ -1050,7 +1090,7 @@
         <f>IF(D47="", "", SUM(D$3:D47))</f>
         <v/>
       </c>
-      <c r="F47" s="10"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
@@ -1060,7 +1100,7 @@
         <f>IF(D48="", "", SUM(D$3:D48))</f>
         <v/>
       </c>
-      <c r="F48" s="10"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
@@ -1070,7 +1110,7 @@
         <f>IF(D49="", "", SUM(D$3:D49))</f>
         <v/>
       </c>
-      <c r="F49" s="10"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
@@ -1080,7 +1120,7 @@
         <f>IF(D50="", "", SUM(D$3:D50))</f>
         <v/>
       </c>
-      <c r="F50" s="10"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
@@ -1090,7 +1130,7 @@
         <f>IF(D51="", "", SUM(D$3:D51))</f>
         <v/>
       </c>
-      <c r="F51" s="10"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
@@ -1100,7 +1140,7 @@
         <f>IF(D52="", "", SUM(D$3:D52))</f>
         <v/>
       </c>
-      <c r="F52" s="10"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
@@ -1110,7 +1150,7 @@
         <f>IF(D53="", "", SUM(D$3:D53))</f>
         <v/>
       </c>
-      <c r="F53" s="10"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
@@ -1120,7 +1160,7 @@
         <f>IF(D54="", "", SUM(D$3:D54))</f>
         <v/>
       </c>
-      <c r="F54" s="10"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
@@ -1130,7 +1170,7 @@
         <f>IF(D55="", "", SUM(D$3:D55))</f>
         <v/>
       </c>
-      <c r="F55" s="10"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
@@ -1140,7 +1180,7 @@
         <f>IF(D56="", "", SUM(D$3:D56))</f>
         <v/>
       </c>
-      <c r="F56" s="10"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="2:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
@@ -2583,8 +2623,11 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added weapons gameobjects instantiation
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Created Item.cs, Weapon.cs, Sword.cs, Bow.cs, Staff.cs and Arrow.cs (Fully functional)</t>
+  </si>
+  <si>
+    <t>Added weapons gameObject instantiation</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,9 +230,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -251,13 +251,13 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -572,7 +572,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -616,17 +616,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>1</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f>SUM(D3:D5)</f>
         <v>3.5</v>
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>14.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -637,10 +637,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -651,10 +651,10 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>3.5</v>
       </c>
-      <c r="F5" s="22"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="15">
         <v>42312</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -673,7 +673,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -703,12 +703,16 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="str">
+      <c r="B9" s="13"/>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="1">
         <f>IF(D9="", "", SUM(D$3:D9))</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -2623,11 +2627,12 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Worked on Inventory (not working yet) + separated arrow's visual and logic
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Added weapons gameObject instantiation</t>
+  </si>
+  <si>
+    <t>Worked on Inventory</t>
+  </si>
+  <si>
+    <t>Separated visual and logic for Arrow, thus creating VisualArrow and Arrow</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -258,6 +264,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +631,7 @@
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,7 +709,10 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>14.5</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="17">
+        <f>SUM(D8:D10)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13"/>
@@ -714,25 +726,35 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>15</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="str">
+      <c r="B10" s="14"/>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="1">
         <f>IF(D10="", "", SUM(D$3:D10))</f>
-        <v/>
-      </c>
-      <c r="F10" s="8"/>
+        <v>16.5</v>
+      </c>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="str">
+      <c r="B11" s="22">
+        <v>42314</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="1">
         <f>IF(D11="", "", SUM(D$3:D11))</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="F11" s="8"/>
     </row>
@@ -2627,12 +2649,13 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="F8:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added health bar + floating damages/heals
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Finished InventoryPanel behaviour</t>
+  </si>
+  <si>
+    <t>Added healthBar and floating damages/heals</t>
   </si>
 </sst>
 </file>
@@ -239,6 +242,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -246,9 +255,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -267,9 +273,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -584,7 +587,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +618,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="14">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -628,17 +631,17 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>1</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="18">
         <f>SUM(D3:D5)</f>
         <v>3.5</v>
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -649,10 +652,10 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>3</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
@@ -663,10 +666,10 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>3.5</v>
       </c>
-      <c r="F5" s="19"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15">
+      <c r="B6" s="13">
         <v>42312</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -679,13 +682,13 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>9.5</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="21">
         <f>SUM(D6:D7)</f>
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -696,10 +699,10 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>10.5</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="14">
         <v>42313</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -712,13 +715,13 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>14.5</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="18">
         <f>SUM(D8:D10)</f>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -729,10 +732,10 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>15</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="14"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
@@ -743,10 +746,10 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>16.5</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="15">
+      <c r="B11" s="13">
         <v>42314</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -762,7 +765,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
@@ -776,12 +779,18 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="str">
+      <c r="B13" s="12">
+        <v>42315</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
         <f>IF(D13="", "", SUM(D$3:D13))</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="F13" s="8"/>
     </row>

</xml_diff>

<commit_message>
Added floating health bar when npcs are damaged
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Added healthBar and floating damages/heals</t>
+  </si>
+  <si>
+    <t>Added floating health bars when npcs are damaged</t>
   </si>
 </sst>
 </file>
@@ -207,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,10 +245,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -255,9 +258,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -587,7 +587,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,13 +631,13 @@
         <f>IF(D3="", "", SUM(D$3:D3))</f>
         <v>1</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f>SUM(D3:D5)</f>
         <v>3.5</v>
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>20</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <f>IF(D4="", "", SUM(D$3:D4))</f>
         <v>3</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="16"/>
@@ -666,10 +666,10 @@
         <f>IF(D5="", "", SUM(D$3:D5))</f>
         <v>3.5</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>42312</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -682,13 +682,13 @@
         <f>IF(D6="", "", SUM(D$3:D6))</f>
         <v>9.5</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <f>SUM(D6:D7)</f>
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -699,7 +699,7 @@
         <f>IF(D7="", "", SUM(D$3:D7))</f>
         <v>10.5</v>
       </c>
-      <c r="F7" s="22"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
@@ -715,7 +715,7 @@
         <f>IF(D8="", "", SUM(D$3:D8))</f>
         <v>14.5</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <f>SUM(D8:D10)</f>
         <v>6</v>
       </c>
@@ -732,7 +732,7 @@
         <f>IF(D9="", "", SUM(D$3:D9))</f>
         <v>15</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
@@ -746,10 +746,10 @@
         <f>IF(D10="", "", SUM(D$3:D10))</f>
         <v>16.5</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>42314</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -765,7 +765,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
@@ -779,7 +779,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+      <c r="B13" s="14">
         <v>42315</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -795,12 +795,16 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="str">
+      <c r="B14" s="15"/>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="1">
         <f>IF(D14="", "", SUM(D$3:D14))</f>
-        <v/>
+        <v>21.5</v>
       </c>
       <c r="F14" s="8"/>
     </row>
@@ -2665,7 +2669,8 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>

</xml_diff>

<commit_message>
Added death ragdoll + enemy behaviour (attack on sight and die) + added GameOver text Log
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Added floating health bars when npcs are damaged</t>
+  </si>
+  <si>
+    <t>Added death ragdoll effect + enemy behaviour (attacking on sight)</t>
   </si>
 </sst>
 </file>
@@ -245,16 +248,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +621,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -637,11 +640,11 @@
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -669,7 +672,7 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="B6" s="14">
         <v>42312</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -688,7 +691,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -702,7 +705,7 @@
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+      <c r="B8" s="12">
         <v>42313</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -721,7 +724,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -749,7 +752,7 @@
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="B11" s="14">
         <v>42314</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -765,7 +768,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
@@ -779,7 +782,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>42315</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -795,7 +798,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
@@ -809,12 +812,16 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="str">
+      <c r="B15" s="13"/>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
         <f>IF(D15="", "", SUM(D$3:D15))</f>
-        <v/>
+        <v>22.5</v>
       </c>
       <c r="F15" s="8"/>
     </row>
@@ -2670,7 +2677,6 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
@@ -2678,6 +2684,7 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="F8:F10"/>
+    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed various issues related to characters death and enemies update
- Now hitting dead characters will make them fly away without triggering
OnDeath
- Fixed an issue where dead character's navmeshagents were reactivated
when selecting another hero
- Disabled NPC's healthbars when opening menus
- Enemies started with destination at 0,0,0; now fixed
</commit_message>
<xml_diff>
--- a/Time tracking.xlsx
+++ b/Time tracking.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Added death ragdoll effect + enemy behaviour (attacking on sight)</t>
+  </si>
+  <si>
+    <t>Fixed various issues related to characters death and enemy update</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -248,16 +251,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -276,6 +279,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -590,7 +596,7 @@
   <dimension ref="B2:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +627,7 @@
       </c>
     </row>
     <row r="3" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="14">
         <v>42311</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -640,11 +646,11 @@
       </c>
       <c r="G3" s="7">
         <f>SUM(D3:D200)</f>
-        <v>22.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
@@ -672,7 +678,7 @@
       <c r="F5" s="19"/>
     </row>
     <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+      <c r="B6" s="12">
         <v>42312</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -691,7 +697,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
@@ -705,7 +711,7 @@
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="14">
         <v>42313</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -724,7 +730,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
@@ -752,7 +758,7 @@
       <c r="F10" s="18"/>
     </row>
     <row r="11" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>42314</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -765,10 +771,13 @@
         <f>IF(D11="", "", SUM(D$3:D11))</f>
         <v>17</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="20">
+        <f>SUM(D11:D12)</f>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="12" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
@@ -779,10 +788,10 @@
         <f>IF(D12="", "", SUM(D$3:D12))</f>
         <v>18</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12">
+      <c r="B13" s="14">
         <v>42315</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -795,10 +804,13 @@
         <f>IF(D13="", "", SUM(D$3:D13))</f>
         <v>20</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="17">
+        <f>SUM(D13:D15)</f>
+        <v>4.5</v>
+      </c>
     </row>
     <row r="14" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
@@ -809,10 +821,10 @@
         <f>IF(D14="", "", SUM(D$3:D14))</f>
         <v>21.5</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="18"/>
     </row>
     <row r="15" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="13"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="4" t="s">
         <v>18</v>
       </c>
@@ -823,15 +835,21 @@
         <f>IF(D15="", "", SUM(D$3:D15))</f>
         <v>22.5</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="str">
+      <c r="B16" s="22">
+        <v>42317</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="1">
         <f>IF(D16="", "", SUM(D$3:D16))</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="F16" s="8"/>
     </row>
@@ -2676,7 +2694,10 @@
       <c r="F200" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F15"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B7"/>
@@ -2684,7 +2705,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="F8:F10"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>